<commit_message>
added charts of distributions and readme file with overview of the project
</commit_message>
<xml_diff>
--- a/symulacja.xlsx
+++ b/symulacja.xlsx
@@ -476,17 +476,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>67.15%</t>
+          <t>67.23%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>95.31%</t>
+          <t>95.35%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>99.12%</t>
+          <t>99.09%</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -500,21 +500,21 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49</v>
+        <v>48.9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30.78%</t>
+          <t>30.68%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>86.58%</t>
+          <t>86.59%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>96.72%</t>
+          <t>96.73%</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -528,21 +528,21 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40.6</v>
+        <v>40.7</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.04%</t>
+          <t>1.06%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9.08%</t>
+          <t>9.11%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>48.03%</t>
+          <t>48.23%</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -560,17 +560,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.78%</t>
+          <t>0.79%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.33%</t>
+          <t>6.25%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>34.71%</t>
+          <t>34.61%</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -588,17 +588,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.25%</t>
+          <t>0.24%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.53%</t>
+          <t>2.52%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>18.33%</t>
+          <t>18.23%</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -621,12 +621,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.11%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.69%</t>
+          <t>1.74%</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -654,7 +654,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.19%</t>
+          <t>1.13%</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -682,7 +682,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.19%</t>
+          <t>0.23%</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -710,7 +710,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0.01%</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0.01%</t>
         </is>
       </c>
       <c r="F11" t="n">

</xml_diff>